<commit_message>
Master Data Definition File Update
</commit_message>
<xml_diff>
--- a/MasterDataFile_DataDictionary_v1_072723.xlsx
+++ b/MasterDataFile_DataDictionary_v1_072723.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cnmc-my.sharepoint.com/personal/rpodolsky_childrensnational_org/Documents/Documents/GitHub/ACHD_PCORNet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="8_{1FDD4EF7-D287-420D-B1B3-B8B6AA922A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B4667CA-F22D-4AD0-9C12-CABCFE02E24C}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{1FDD4EF7-D287-420D-B1B3-B8B6AA922A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDA9F6B0-6D6C-4A70-975A-BC69D672B7BE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{B23E0A7E-91BC-4D0A-A7AE-634991F558D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B23E0A7E-91BC-4D0A-A7AE-634991F558D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
   <si>
     <t>Variable Name</t>
   </si>
@@ -2533,15 +2533,6 @@
     </r>
   </si>
   <si>
-    <t>OUTPATIENT_VISITS</t>
-  </si>
-  <si>
-    <t>Outpatient Visit N</t>
-  </si>
-  <si>
-    <t>Counts of encounters per patient that had ENCOUNTER.ENCOUNTER_TYPE="AV" or…</t>
-  </si>
-  <si>
     <t>Primary CHD Diagnosis determined based on a diagnosis hierarchy. The primary CHD diagnosis is the diagnosis a patient (PATID) has that is highest in hierarchy.</t>
   </si>
   <si>
@@ -2567,6 +2558,37 @@
   </si>
   <si>
     <t>All lab concepts</t>
+  </si>
+  <si>
+    <t>OUTPATIENT_VISIT_N</t>
+  </si>
+  <si>
+    <t>Outpatient Visit Number</t>
+  </si>
+  <si>
+    <t>MACRO_VISIT_TYPE</t>
+  </si>
+  <si>
+    <t>Macro Visit Type</t>
+  </si>
+  <si>
+    <t>CHAR(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three types of macro visit:
+OP = Outpatient
+ED = Emergency Department
+IP = Inpatient
+Logic: 
+1.	Generate macro-visits as all encounters except for ENC_TYPE = OA with overlapping ADMIT_DATE and MV_DISCHARGE_DATE. 
+•	All encounters except those with ENCOUNTER_TYPE=ED: MV_DISCHARGE_DATE = DISCHARGE_DATE.
+•	All encounters with ENCOUNTER_TYPE=ED: MV_DISCHARGE_DATE=min(DISCHARGE_DATE, ADMIT_DATE + 2 days). 
+2.	IP macro visit = any macro visit that has an encounter with ENC_TYPE in IP or EI or an encounter with ENC_TYPE=ED and DISCHARGE_STATUS=IP within the macro visit regardless of ENC_TYPE for other encounters within the macro-visit. 
+3.	ED macro visit = any macro-visit that is NOT an IP macro visit AND that has at least one encounter with ENC_TYPE in ED or OS. 
+4.	OP macro visit = any macro visit that is NOT an ED macro visit AND that has at least one encounter with ENC_TYPE in AV or TH regardless of ENC_TYPE for other encounters. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counts of MACRO_VISITS_TYPE="OP" </t>
   </si>
 </sst>
 </file>
@@ -2768,7 +2790,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2805,6 +2827,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2817,8 +2842,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3135,10 +3160,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E896B3B-F48C-4D31-AFC5-874D4B891D00}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3222,8 +3247,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>71</v>
+      <c r="A5" s="14" t="s">
+        <v>68</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>16</v>
@@ -3234,16 +3259,16 @@
       <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="186.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>70</v>
+      <c r="A6" s="14" t="s">
+        <v>67</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>21</v>
@@ -3254,8 +3279,8 @@
       <c r="D6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="17"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:6" ht="382.5" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
@@ -3417,15 +3442,29 @@
       </c>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="285" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>69</v>
+        <v>79</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3442,7 +3481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33BD1D51-ACAC-4351-B7FB-EEEAA68A3B92}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3454,34 +3493,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>77</v>
+        <v>73</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>